<commit_message>
File structure and BOM update
</commit_message>
<xml_diff>
--- a/Purchasing/Active BOM.xlsx
+++ b/Purchasing/Active BOM.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home03\jtalik\Desktop\github\electric-feed-system\Purchasing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Dropbox\GitHub\electric-feed-system\Purchasing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="106">
   <si>
     <t>Part</t>
   </si>
@@ -347,7 +347,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
@@ -503,26 +503,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -594,9 +576,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -609,9 +588,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -633,16 +609,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,6 +628,37 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1008,1298 +1011,1323 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20:O20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" style="7" customWidth="1"/>
-    <col min="10" max="14" width="3.5703125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" style="7" customWidth="1"/>
-    <col min="16" max="175" width="14.42578125" customWidth="1"/>
-    <col min="176" max="1025" width="14.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="35.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.73046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" style="1" customWidth="1"/>
+    <col min="10" max="14" width="3.59765625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.796875" style="1" customWidth="1"/>
+    <col min="16" max="175" width="14.3984375" customWidth="1"/>
+    <col min="176" max="1025" width="14.3984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-    </row>
-    <row r="2" spans="1:15" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+    </row>
+    <row r="3" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="11">
         <v>54.37</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="12">
         <v>1</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="13">
         <f>B3*C3</f>
         <v>54.37</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="5" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+    </row>
+    <row r="4" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="11">
         <v>54.93</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="12">
         <v>1</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="13">
         <f>B4*C4</f>
         <v>54.93</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="5" t="s">
+      <c r="G4" s="16"/>
+      <c r="H4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+    </row>
+    <row r="5" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="18">
         <v>53.87</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="12">
         <v>1</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="13">
         <f>B5*C5</f>
         <v>53.87</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="5" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+    </row>
+    <row r="6" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-    </row>
-    <row r="7" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+    </row>
+    <row r="7" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="26">
         <v>6.72</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="13">
         <f t="shared" ref="D7:D19" si="0">B7*C7</f>
         <v>6.72</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="36" t="s">
+      <c r="G7" s="28"/>
+      <c r="H7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+    </row>
+    <row r="8" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="30">
         <v>29.94</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="31">
         <v>1</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="13">
         <f t="shared" si="0"/>
         <v>29.94</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="G8" s="28"/>
+      <c r="H8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="29"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+    </row>
+    <row r="9" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="26">
         <v>6.87</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="12">
         <v>2</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="13">
         <f t="shared" si="0"/>
         <v>13.74</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="G9" s="28"/>
+      <c r="H9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="29"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+    </row>
+    <row r="10" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="26">
         <v>17.12</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="12">
         <v>2</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="13">
         <f t="shared" si="0"/>
         <v>34.24</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="36" t="s">
+      <c r="G10" s="28"/>
+      <c r="H10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+    </row>
+    <row r="11" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="26">
         <v>4.04</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="12">
         <v>2</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="13">
         <f t="shared" si="0"/>
         <v>8.08</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="36" t="s">
+      <c r="G11" s="28"/>
+      <c r="H11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+    </row>
+    <row r="12" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="26">
         <v>8.11</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="12">
         <v>2</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="13">
         <f t="shared" si="0"/>
         <v>16.22</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="35"/>
-      <c r="H12" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
+      <c r="G12" s="28"/>
+      <c r="H12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="29"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+    </row>
+    <row r="13" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="26">
         <v>3.68</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="12">
         <v>1</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="13">
         <f t="shared" si="0"/>
         <v>3.68</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="35"/>
-      <c r="H13" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="5" t="s">
+      <c r="G13" s="28"/>
+      <c r="H13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="29"/>
+      <c r="J13" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+    </row>
+    <row r="14" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="26">
         <v>6.01</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="12">
         <v>1</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="13">
         <f t="shared" si="0"/>
         <v>6.01</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="35"/>
-      <c r="H14" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="36"/>
-      <c r="J14" s="5" t="s">
+      <c r="G14" s="28"/>
+      <c r="H14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="29"/>
+      <c r="J14" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+    </row>
+    <row r="15" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="26">
         <v>9.77</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="12">
         <v>1</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="13">
         <f t="shared" si="0"/>
         <v>9.77</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="5" t="s">
+      <c r="G15" s="28"/>
+      <c r="H15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="29"/>
+      <c r="J15" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+    </row>
+    <row r="16" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="33">
+      <c r="B16" s="26">
         <v>5.7</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="12">
         <v>3</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="13">
         <f t="shared" si="0"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="36"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
+      <c r="G16" s="28"/>
+      <c r="H16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="29"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+    </row>
+    <row r="17" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="26">
         <v>20.7</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="12">
         <v>2</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="13">
         <f t="shared" si="0"/>
         <v>41.4</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="35"/>
-      <c r="H17" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="36"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
+      <c r="G17" s="28"/>
+      <c r="H17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="29"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+    </row>
+    <row r="18" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="26">
         <v>5.68</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="12">
         <v>2</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="13">
         <f t="shared" si="0"/>
         <v>11.36</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F18" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="35"/>
-      <c r="H18" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
+      <c r="G18" s="28"/>
+      <c r="H18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="29"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="47"/>
+    </row>
+    <row r="19" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="11">
         <v>2.6</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="31">
         <v>3</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="13">
         <f t="shared" si="0"/>
         <v>7.8000000000000007</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="35"/>
-      <c r="H19" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="36" t="s">
+      <c r="G19" s="28"/>
+      <c r="H19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37" t="s">
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+    </row>
+    <row r="20" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="11">
         <v>25.93</v>
       </c>
-      <c r="C20" s="39">
+      <c r="C20" s="31">
         <v>1</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="13">
         <f t="shared" ref="D20" si="1">B20*C20</f>
         <v>25.93</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="36" t="s">
+      <c r="G20" s="44"/>
+      <c r="H20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-    </row>
-    <row r="21" spans="1:15" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+    </row>
+    <row r="21" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A21" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-    </row>
-    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+    </row>
+    <row r="22" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="11">
         <v>97.89</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="12">
         <v>1</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="13">
         <f>B22*C22</f>
         <v>97.89</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="12">
         <v>9052000029</v>
       </c>
-      <c r="G22" s="43"/>
-      <c r="H22" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="44" t="str">
+      <c r="G22" s="35"/>
+      <c r="H22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="36" t="str">
         <f>HYPERLINK("https://hobbyking.com/en_us/turnigy-aquastar-t20-3t-730kv-1280kv-water-cooled-brushless-motor.html?___store=en_us","https://hobbyking.com/en_us/turnigy-aquastar-t20-3t-730kv-1280kv-water-cooled-brushless-motor.html?___store=en_us")</f>
         <v>https://hobbyking.com/en_us/turnigy-aquastar-t20-3t-730kv-1280kv-water-cooled-brushless-motor.html?___store=en_us</v>
       </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="45"/>
+    </row>
+    <row r="23" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="11">
         <v>247.07</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="12">
         <v>1</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="13">
         <f>B23*C23</f>
         <v>247.07</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="43"/>
-      <c r="H23" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="44" t="s">
+      <c r="G23" s="35"/>
+      <c r="H23" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="45"/>
+    </row>
+    <row r="24" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="11">
         <v>3.5</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="12">
         <v>2</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="13">
         <f>B24*C24</f>
         <v>7</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="44" t="s">
+      <c r="G24" s="35"/>
+      <c r="H24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="45"/>
+    </row>
+    <row r="25" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="11">
         <v>18</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="12">
         <v>1</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="13">
         <f>B25*C25</f>
         <v>18</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="43"/>
-      <c r="H25" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="44" t="s">
+      <c r="G25" s="35"/>
+      <c r="H25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="45"/>
+    </row>
+    <row r="26" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="11">
         <v>157.57</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="12">
         <v>2</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="13">
         <f>B26*C26</f>
         <v>315.14</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G26" s="43"/>
-      <c r="H26" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="44" t="s">
+      <c r="G26" s="35"/>
+      <c r="H26" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-    </row>
-    <row r="27" spans="1:15" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="45" t="s">
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="45"/>
+    </row>
+    <row r="27" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A27" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="49"/>
+    </row>
+    <row r="28" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18">
+      <c r="B28" s="11"/>
+      <c r="C28" s="12">
         <v>1</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="13">
         <f t="shared" ref="D28:D33" si="2">B28*C28</f>
         <v>0</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F28" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="46"/>
-      <c r="H28" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="23"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+      <c r="G28" s="37"/>
+      <c r="H28" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="45"/>
+      <c r="O28" s="45"/>
+    </row>
+    <row r="29" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18">
+      <c r="B29" s="11"/>
+      <c r="C29" s="12">
         <v>1</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F29" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="46"/>
-      <c r="H29" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="23"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
+      <c r="G29" s="37"/>
+      <c r="H29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+    </row>
+    <row r="30" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A30" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18">
+      <c r="B30" s="11"/>
+      <c r="C30" s="12">
         <v>1</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="18" t="s">
+      <c r="E30" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="G30" s="46"/>
-      <c r="H30" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="23"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-    </row>
-    <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
+      <c r="G30" s="37"/>
+      <c r="H30" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="17"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
+    </row>
+    <row r="31" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18">
+      <c r="B31" s="11"/>
+      <c r="C31" s="12">
         <v>1</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G31" s="46"/>
-      <c r="H31" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="23"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
+      <c r="G31" s="37"/>
+      <c r="H31" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="17"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+    </row>
+    <row r="32" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18">
+      <c r="B32" s="11"/>
+      <c r="C32" s="12">
         <v>1</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F32" s="18" t="s">
+      <c r="F32" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G32" s="46"/>
-      <c r="H32" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="23"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
+      <c r="G32" s="37"/>
+      <c r="H32" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="17"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+    </row>
+    <row r="33" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A33" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="18">
+      <c r="B33" s="11"/>
+      <c r="C33" s="12">
         <v>1</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G33" s="46"/>
-      <c r="H33" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" s="23"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-    </row>
-    <row r="34" spans="1:15" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="45" t="s">
+      <c r="G33" s="37"/>
+      <c r="H33" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="17"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="45"/>
+      <c r="O33" s="45"/>
+    </row>
+    <row r="34" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A34" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+    </row>
+    <row r="35" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35" s="11">
         <v>13.54</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="12">
         <v>1</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="13">
         <f>B35*C35</f>
         <v>13.54</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F35" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G35" s="22"/>
-      <c r="H35" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="44" t="s">
+      <c r="G35" s="16"/>
+      <c r="H35" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-    </row>
-    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="47"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19">
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="45"/>
+      <c r="O35" s="45"/>
+    </row>
+    <row r="36" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="38"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="13">
         <f>B36*C36</f>
         <v>0</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="23"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-    </row>
-    <row r="37" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="47"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19">
+      <c r="E36" s="17"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="17"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="45"/>
+      <c r="N36" s="45"/>
+      <c r="O36" s="45"/>
+    </row>
+    <row r="37" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="38"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="13">
         <f>B37*C37</f>
         <v>0</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-    </row>
-    <row r="38" spans="1:15" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="45" t="s">
+      <c r="E37" s="17"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="48"/>
+      <c r="O37" s="48"/>
+    </row>
+    <row r="38" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A38" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-    </row>
-    <row r="39" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="16" t="s">
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+    </row>
+    <row r="39" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="11">
         <v>7.8</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="12">
         <v>100</v>
       </c>
-      <c r="D39" s="19">
+      <c r="D39" s="13">
         <f>B39*C39/100</f>
         <v>7.8</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F39" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="G39" s="46"/>
-      <c r="H39" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I39" s="44" t="s">
+      <c r="G39" s="37"/>
+      <c r="H39" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-    </row>
-    <row r="40" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="45"/>
+      <c r="N39" s="45"/>
+      <c r="O39" s="45"/>
+    </row>
+    <row r="40" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B40" s="17">
+      <c r="B40" s="11">
         <v>6</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="12">
         <v>100</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D40" s="13">
         <f>B40*C40/5</f>
         <v>120</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="G40" s="46"/>
-      <c r="H40" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="44" t="s">
+      <c r="G40" s="37"/>
+      <c r="H40" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="45"/>
+      <c r="N40" s="45"/>
+      <c r="O40" s="45"/>
+    </row>
+    <row r="41" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="11">
         <v>4.83</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="12">
         <v>2</v>
       </c>
-      <c r="D41" s="19">
+      <c r="D41" s="13">
         <f>B41*C41/5</f>
         <v>1.9319999999999999</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F41" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="46"/>
-      <c r="H41" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I41" s="44" t="s">
+      <c r="G41" s="37"/>
+      <c r="H41" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="1:15" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="48" t="s">
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="45"/>
+      <c r="M41" s="45"/>
+      <c r="N41" s="45"/>
+      <c r="O41" s="45"/>
+    </row>
+    <row r="42" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A42" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="49"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="50"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="46"/>
+      <c r="N42" s="46"/>
+      <c r="O42" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="J11:O11"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="J15:O15"/>
+    <mergeCell ref="J16:O16"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="J24:O24"/>
     <mergeCell ref="J40:O40"/>
     <mergeCell ref="J41:O41"/>
     <mergeCell ref="J42:O42"/>
@@ -2316,29 +2344,6 @@
     <mergeCell ref="J34:O34"/>
     <mergeCell ref="J25:O25"/>
     <mergeCell ref="J26:O26"/>
-    <mergeCell ref="J27:O27"/>
-    <mergeCell ref="J28:O28"/>
-    <mergeCell ref="J29:O29"/>
-    <mergeCell ref="J18:O18"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="J22:O22"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="J15:O15"/>
-    <mergeCell ref="J16:O16"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J7:O7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I7" r:id="rId1" location="90967A160"/>
@@ -2355,6 +2360,6 @@
     <hyperlink ref="I41" r:id="rId12" location="91290a172/=175py34"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add boring bar to be ordered to BOM
</commit_message>
<xml_diff>
--- a/Purchasing/Active BOM.xlsx
+++ b/Purchasing/Active BOM.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Dropbox\GitHub\electric-feed-system\Purchasing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\electric-feed-system\Purchasing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="110">
   <si>
     <t>Part</t>
   </si>
@@ -342,18 +342,30 @@
   </si>
   <si>
     <t>used as the initial seal</t>
+  </si>
+  <si>
+    <t>Micro boring bar</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Micro 100 QBB-1801500</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Micro-100-BB-1801500-Diameter-Projection/dp/B00Q8KO22S/ref=pd_day0_328_1?_encoding=UTF8&amp;pd_rd_i=B00Q8KO22S&amp;pd_rd_r=7ZD38H4CKCTA07TWZ87K&amp;pd_rd_w=Dnyxf&amp;pd_rd_wg=Pl77d&amp;psc=1&amp;refRID=7ZD38H4CKCTA07TWZ87K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="\$#,##0.00\ ;[Red]&quot;($&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -415,6 +427,17 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -503,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -629,24 +652,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -660,6 +665,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1009,30 +1040,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK42"/>
+  <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.86328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.73046875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" style="1" customWidth="1"/>
-    <col min="10" max="14" width="3.59765625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.796875" style="1" customWidth="1"/>
-    <col min="16" max="175" width="14.3984375" customWidth="1"/>
-    <col min="176" max="1025" width="14.3984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
+    <col min="10" max="14" width="3.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" style="1" customWidth="1"/>
+    <col min="16" max="175" width="14.42578125" customWidth="1"/>
+    <col min="176" max="1025" width="14.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1100,7 @@
       <c r="N1" s="50"/>
       <c r="O1" s="50"/>
     </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1088,7 +1119,7 @@
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
@@ -1113,16 +1144,16 @@
         <v>14</v>
       </c>
       <c r="I3" s="17"/>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-    </row>
-    <row r="4" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
@@ -1147,16 +1178,16 @@
         <v>14</v>
       </c>
       <c r="I4" s="17"/>
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-    </row>
-    <row r="5" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
@@ -1181,17 +1212,17 @@
         <v>14</v>
       </c>
       <c r="I5" s="17"/>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-    </row>
-    <row r="6" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" s="51" t="s">
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+    </row>
+    <row r="6" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="45" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="20"/>
@@ -1209,8 +1240,8 @@
       <c r="N6" s="24"/>
       <c r="O6" s="24"/>
     </row>
-    <row r="7" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="54" t="s">
+    <row r="7" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="48" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="26">
@@ -1236,17 +1267,17 @@
       <c r="I7" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="47" t="s">
+      <c r="J7" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-    </row>
-    <row r="8" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="55" t="s">
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+    </row>
+    <row r="8" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="30">
@@ -1270,15 +1301,15 @@
         <v>14</v>
       </c>
       <c r="I8" s="29"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-    </row>
-    <row r="9" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="55" t="s">
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+    </row>
+    <row r="9" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="49" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="26">
@@ -1302,15 +1333,15 @@
         <v>14</v>
       </c>
       <c r="I9" s="29"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-    </row>
-    <row r="10" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="55" t="s">
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+    </row>
+    <row r="10" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="49" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="26">
@@ -1336,15 +1367,15 @@
       <c r="I10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-    </row>
-    <row r="11" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="55" t="s">
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+    </row>
+    <row r="11" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="49" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="26">
@@ -1370,17 +1401,17 @@
       <c r="I11" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="47" t="s">
+      <c r="J11" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-    </row>
-    <row r="12" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="55" t="s">
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+    </row>
+    <row r="12" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="49" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="26">
@@ -1404,15 +1435,15 @@
         <v>14</v>
       </c>
       <c r="I12" s="29"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-    </row>
-    <row r="13" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="55" t="s">
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+    </row>
+    <row r="13" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="49" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="26">
@@ -1436,17 +1467,17 @@
         <v>14</v>
       </c>
       <c r="I13" s="29"/>
-      <c r="J13" s="47" t="s">
+      <c r="J13" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-    </row>
-    <row r="14" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="55" t="s">
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+    </row>
+    <row r="14" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="49" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="26">
@@ -1470,17 +1501,17 @@
         <v>14</v>
       </c>
       <c r="I14" s="29"/>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-    </row>
-    <row r="15" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="55" t="s">
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+    </row>
+    <row r="15" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="49" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="26">
@@ -1504,17 +1535,17 @@
         <v>14</v>
       </c>
       <c r="I15" s="29"/>
-      <c r="J15" s="47" t="s">
+      <c r="J15" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
-    </row>
-    <row r="16" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="55" t="s">
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
+    </row>
+    <row r="16" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="49" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="26">
@@ -1538,15 +1569,15 @@
         <v>14</v>
       </c>
       <c r="I16" s="29"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
-    </row>
-    <row r="17" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="55" t="s">
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+    </row>
+    <row r="17" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="49" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="26">
@@ -1570,15 +1601,15 @@
         <v>14</v>
       </c>
       <c r="I17" s="29"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="47"/>
-    </row>
-    <row r="18" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="55" t="s">
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+    </row>
+    <row r="18" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="49" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="26">
@@ -1602,15 +1633,15 @@
         <v>14</v>
       </c>
       <c r="I18" s="29"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-    </row>
-    <row r="19" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="55" t="s">
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="51"/>
+    </row>
+    <row r="19" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="49" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="11">
@@ -1636,15 +1667,15 @@
       <c r="I19" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-    </row>
-    <row r="20" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="55" t="s">
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+    </row>
+    <row r="20" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="49" t="s">
         <v>102</v>
       </c>
       <c r="B20" s="11">
@@ -1670,17 +1701,17 @@
       <c r="I20" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="J20" s="47" t="s">
+      <c r="J20" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-    </row>
-    <row r="21" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
-      <c r="A21" s="51" t="s">
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+    </row>
+    <row r="21" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="45" t="s">
         <v>57</v>
       </c>
       <c r="B21" s="33"/>
@@ -1698,7 +1729,7 @@
       <c r="N21" s="19"/>
       <c r="O21" s="19"/>
     </row>
-    <row r="22" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>58</v>
       </c>
@@ -1726,14 +1757,14 @@
         <f>HYPERLINK("https://hobbyking.com/en_us/turnigy-aquastar-t20-3t-730kv-1280kv-water-cooled-brushless-motor.html?___store=en_us","https://hobbyking.com/en_us/turnigy-aquastar-t20-3t-730kv-1280kv-water-cooled-brushless-motor.html?___store=en_us")</f>
         <v>https://hobbyking.com/en_us/turnigy-aquastar-t20-3t-730kv-1280kv-water-cooled-brushless-motor.html?___store=en_us</v>
       </c>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-    </row>
-    <row r="23" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
+    </row>
+    <row r="23" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>60</v>
       </c>
@@ -1760,14 +1791,14 @@
       <c r="I23" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="45"/>
-    </row>
-    <row r="24" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
+    </row>
+    <row r="24" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>63</v>
       </c>
@@ -1794,14 +1825,14 @@
       <c r="I24" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="45"/>
-    </row>
-    <row r="25" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="53"/>
+    </row>
+    <row r="25" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>66</v>
       </c>
@@ -1828,14 +1859,14 @@
       <c r="I25" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-    </row>
-    <row r="26" spans="1:15" ht="23.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
+    </row>
+    <row r="26" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>69</v>
       </c>
@@ -1862,15 +1893,15 @@
       <c r="I26" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-    </row>
-    <row r="27" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
-      <c r="A27" s="52" t="s">
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="53"/>
+    </row>
+    <row r="27" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="46" t="s">
         <v>72</v>
       </c>
       <c r="B27" s="20"/>
@@ -1881,18 +1912,18 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="23"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49"/>
-    </row>
-    <row r="28" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="52"/>
+    </row>
+    <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="11"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="12">
         <v>1</v>
       </c>
@@ -1911,18 +1942,18 @@
         <v>14</v>
       </c>
       <c r="I28" s="17"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-    </row>
-    <row r="29" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="53"/>
+    </row>
+    <row r="29" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="11"/>
+      <c r="B29" s="56"/>
       <c r="C29" s="12">
         <v>1</v>
       </c>
@@ -1941,18 +1972,18 @@
         <v>14</v>
       </c>
       <c r="I29" s="17"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-    </row>
-    <row r="30" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+    </row>
+    <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="11"/>
+      <c r="B30" s="56"/>
       <c r="C30" s="12">
         <v>1</v>
       </c>
@@ -1971,18 +2002,18 @@
         <v>14</v>
       </c>
       <c r="I30" s="17"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
-    </row>
-    <row r="31" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="55"/>
+    </row>
+    <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="11"/>
+      <c r="B31" s="56"/>
       <c r="C31" s="12">
         <v>1</v>
       </c>
@@ -2001,18 +2032,18 @@
         <v>14</v>
       </c>
       <c r="I31" s="17"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-    </row>
-    <row r="32" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="53"/>
+    </row>
+    <row r="32" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="11"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="12">
         <v>1</v>
       </c>
@@ -2031,18 +2062,18 @@
         <v>14</v>
       </c>
       <c r="I32" s="17"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-    </row>
-    <row r="33" spans="1:15" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="53"/>
+      <c r="N32" s="53"/>
+      <c r="O32" s="53"/>
+    </row>
+    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="11"/>
+      <c r="B33" s="56"/>
       <c r="C33" s="12">
         <v>1</v>
       </c>
@@ -2061,15 +2092,15 @@
         <v>14</v>
       </c>
       <c r="I33" s="17"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
-    </row>
-    <row r="34" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
-      <c r="A34" s="52" t="s">
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="53"/>
+      <c r="N33" s="53"/>
+      <c r="O33" s="53"/>
+    </row>
+    <row r="34" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="46" t="s">
         <v>86</v>
       </c>
       <c r="B34" s="20"/>
@@ -2080,18 +2111,18 @@
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="23"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="49"/>
-      <c r="O34" s="49"/>
-    </row>
-    <row r="35" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="52"/>
+      <c r="M34" s="52"/>
+      <c r="N34" s="52"/>
+      <c r="O34" s="52"/>
+    </row>
+    <row r="35" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B35" s="56">
         <v>13.54</v>
       </c>
       <c r="C35" s="12">
@@ -2114,16 +2145,16 @@
       <c r="I35" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J35" s="45"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="45"/>
-      <c r="O35" s="45"/>
-    </row>
-    <row r="36" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="53"/>
+      <c r="N35" s="53"/>
+      <c r="O35" s="53"/>
+    </row>
+    <row r="36" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="38"/>
-      <c r="B36" s="11"/>
+      <c r="B36" s="56"/>
       <c r="C36" s="12"/>
       <c r="D36" s="13">
         <f>B36*C36</f>
@@ -2136,16 +2167,16 @@
         <v>14</v>
       </c>
       <c r="I36" s="17"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-    </row>
-    <row r="37" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="53"/>
+      <c r="N36" s="53"/>
+      <c r="O36" s="53"/>
+    </row>
+    <row r="37" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="38"/>
-      <c r="B37" s="11"/>
+      <c r="B37" s="56"/>
       <c r="C37" s="12"/>
       <c r="D37" s="13">
         <f>B37*C37</f>
@@ -2156,15 +2187,15 @@
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="17"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
-      <c r="M37" s="48"/>
-      <c r="N37" s="48"/>
-      <c r="O37" s="48"/>
-    </row>
-    <row r="38" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.35">
-      <c r="A38" s="52" t="s">
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="55"/>
+      <c r="M37" s="55"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="55"/>
+    </row>
+    <row r="38" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="46" t="s">
         <v>91</v>
       </c>
       <c r="B38" s="20"/>
@@ -2175,18 +2206,18 @@
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="I38" s="23"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="49"/>
-    </row>
-    <row r="39" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J38" s="52"/>
+      <c r="K38" s="52"/>
+      <c r="L38" s="52"/>
+      <c r="M38" s="52"/>
+      <c r="N38" s="52"/>
+      <c r="O38" s="52"/>
+    </row>
+    <row r="39" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="56">
         <v>7.8</v>
       </c>
       <c r="C39" s="12">
@@ -2209,18 +2240,18 @@
       <c r="I39" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-    </row>
-    <row r="40" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="53"/>
+      <c r="O39" s="53"/>
+    </row>
+    <row r="40" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="56">
         <v>6</v>
       </c>
       <c r="C40" s="12">
@@ -2243,18 +2274,18 @@
       <c r="I40" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="J40" s="45"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="45"/>
-      <c r="N40" s="45"/>
-      <c r="O40" s="45"/>
-    </row>
-    <row r="41" spans="1:15" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="53"/>
+    </row>
+    <row r="41" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="56">
         <v>4.83</v>
       </c>
       <c r="C41" s="12">
@@ -2277,15 +2308,15 @@
       <c r="I41" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
-      <c r="O41" s="45"/>
-    </row>
-    <row r="42" spans="1:15" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.4">
-      <c r="A42" s="53" t="s">
+      <c r="J41" s="53"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="53"/>
+    </row>
+    <row r="42" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="47" t="s">
         <v>101</v>
       </c>
       <c r="B42" s="39"/>
@@ -2296,38 +2327,43 @@
       <c r="G42" s="40"/>
       <c r="H42" s="40"/>
       <c r="I42" s="41"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="46"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="46"/>
-      <c r="N42" s="46"/>
-      <c r="O42" s="46"/>
+      <c r="J42" s="54"/>
+      <c r="K42" s="54"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54"/>
+      <c r="O42" s="54"/>
+    </row>
+    <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="57">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="13">
+        <f>B43*C43</f>
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E43" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43" s="37"/>
+      <c r="H43" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="J15:O15"/>
-    <mergeCell ref="J16:O16"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="J27:O27"/>
-    <mergeCell ref="J28:O28"/>
-    <mergeCell ref="J29:O29"/>
-    <mergeCell ref="J18:O18"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="J22:O22"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="J24:O24"/>
     <mergeCell ref="J40:O40"/>
     <mergeCell ref="J41:O41"/>
     <mergeCell ref="J42:O42"/>
@@ -2344,6 +2380,29 @@
     <mergeCell ref="J34:O34"/>
     <mergeCell ref="J25:O25"/>
     <mergeCell ref="J26:O26"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="J15:O15"/>
+    <mergeCell ref="J16:O16"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="J11:O11"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J7:O7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I7" r:id="rId1" location="90967A160"/>

</xml_diff>

<commit_message>
add diffiser blanks for printing
</commit_message>
<xml_diff>
--- a/Purchasing/Active BOM.xlsx
+++ b/Purchasing/Active BOM.xlsx
@@ -360,10 +360,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="\$#,##0.00\ ;[Red]&quot;($&quot;#,##0.00\)"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -526,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -665,32 +666,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1043,7 +1047,7 @@
   <dimension ref="A1:AMK43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1091,14 +1095,14 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
     </row>
     <row r="2" spans="1:15" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1144,14 +1148,14 @@
         <v>14</v>
       </c>
       <c r="I3" s="17"/>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
     </row>
     <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1178,14 +1182,14 @@
         <v>14</v>
       </c>
       <c r="I4" s="17"/>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
     </row>
     <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -1212,14 +1216,14 @@
         <v>14</v>
       </c>
       <c r="I5" s="17"/>
-      <c r="J5" s="51" t="s">
+      <c r="J5" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
     </row>
     <row r="6" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
@@ -1267,14 +1271,14 @@
       <c r="I7" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="51" t="s">
+      <c r="J7" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
     </row>
     <row r="8" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="49" t="s">
@@ -1301,12 +1305,12 @@
         <v>14</v>
       </c>
       <c r="I8" s="29"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="51"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
     </row>
     <row r="9" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="49" t="s">
@@ -1333,12 +1337,12 @@
         <v>14</v>
       </c>
       <c r="I9" s="29"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
     </row>
     <row r="10" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="49" t="s">
@@ -1367,12 +1371,12 @@
       <c r="I10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
     </row>
     <row r="11" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="49" t="s">
@@ -1401,14 +1405,14 @@
       <c r="I11" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="51" t="s">
+      <c r="J11" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
     </row>
     <row r="12" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="49" t="s">
@@ -1435,12 +1439,12 @@
         <v>14</v>
       </c>
       <c r="I12" s="29"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
     </row>
     <row r="13" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="49" t="s">
@@ -1467,14 +1471,14 @@
         <v>14</v>
       </c>
       <c r="I13" s="29"/>
-      <c r="J13" s="51" t="s">
+      <c r="J13" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
+      <c r="O13" s="54"/>
     </row>
     <row r="14" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="49" t="s">
@@ -1501,14 +1505,14 @@
         <v>14</v>
       </c>
       <c r="I14" s="29"/>
-      <c r="J14" s="51" t="s">
+      <c r="J14" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="54"/>
     </row>
     <row r="15" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="49" t="s">
@@ -1535,14 +1539,14 @@
         <v>14</v>
       </c>
       <c r="I15" s="29"/>
-      <c r="J15" s="51" t="s">
+      <c r="J15" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
     </row>
     <row r="16" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="49" t="s">
@@ -1569,12 +1573,12 @@
         <v>14</v>
       </c>
       <c r="I16" s="29"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
     </row>
     <row r="17" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="49" t="s">
@@ -1601,12 +1605,12 @@
         <v>14</v>
       </c>
       <c r="I17" s="29"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="51"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
     </row>
     <row r="18" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="49" t="s">
@@ -1633,12 +1637,12 @@
         <v>14</v>
       </c>
       <c r="I18" s="29"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="51"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
     </row>
     <row r="19" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
@@ -1667,12 +1671,12 @@
       <c r="I19" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
     </row>
     <row r="20" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="49" t="s">
@@ -1701,14 +1705,14 @@
       <c r="I20" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="J20" s="51" t="s">
+      <c r="J20" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
     </row>
     <row r="21" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21" s="45" t="s">
@@ -1757,12 +1761,12 @@
         <f>HYPERLINK("https://hobbyking.com/en_us/turnigy-aquastar-t20-3t-730kv-1280kv-water-cooled-brushless-motor.html?___store=en_us","https://hobbyking.com/en_us/turnigy-aquastar-t20-3t-730kv-1280kv-water-cooled-brushless-motor.html?___store=en_us")</f>
         <v>https://hobbyking.com/en_us/turnigy-aquastar-t20-3t-730kv-1280kv-water-cooled-brushless-motor.html?___store=en_us</v>
       </c>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="53"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="52"/>
     </row>
     <row r="23" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
@@ -1791,12 +1795,12 @@
       <c r="I23" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="53"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="52"/>
     </row>
     <row r="24" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
@@ -1825,12 +1829,12 @@
       <c r="I24" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="53"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
     </row>
     <row r="25" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
@@ -1859,12 +1863,12 @@
       <c r="I25" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="53"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="52"/>
+      <c r="O25" s="52"/>
     </row>
     <row r="26" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
@@ -1893,12 +1897,12 @@
       <c r="I26" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="52"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="52"/>
     </row>
     <row r="27" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A27" s="46" t="s">
@@ -1912,18 +1916,18 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="23"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="52"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
     </row>
     <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="56"/>
+      <c r="B28" s="59"/>
       <c r="C28" s="12">
         <v>1</v>
       </c>
@@ -1942,18 +1946,18 @@
         <v>14</v>
       </c>
       <c r="I28" s="17"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="53"/>
-      <c r="O28" s="53"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
     </row>
     <row r="29" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="56"/>
+      <c r="B29" s="59"/>
       <c r="C29" s="12">
         <v>1</v>
       </c>
@@ -1972,18 +1976,18 @@
         <v>14</v>
       </c>
       <c r="I29" s="17"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
-      <c r="N29" s="53"/>
-      <c r="O29" s="53"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="52"/>
     </row>
     <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="56"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="12">
         <v>1</v>
       </c>
@@ -2013,7 +2017,7 @@
       <c r="A31" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="56"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="12">
         <v>1</v>
       </c>
@@ -2032,18 +2036,18 @@
         <v>14</v>
       </c>
       <c r="I31" s="17"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="53"/>
-      <c r="N31" s="53"/>
-      <c r="O31" s="53"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52"/>
+      <c r="O31" s="52"/>
     </row>
     <row r="32" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="56"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="12">
         <v>1</v>
       </c>
@@ -2062,18 +2066,18 @@
         <v>14</v>
       </c>
       <c r="I32" s="17"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="53"/>
-      <c r="N32" s="53"/>
-      <c r="O32" s="53"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="52"/>
+      <c r="N32" s="52"/>
+      <c r="O32" s="52"/>
     </row>
     <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="56"/>
+      <c r="B33" s="59"/>
       <c r="C33" s="12">
         <v>1</v>
       </c>
@@ -2092,12 +2096,12 @@
         <v>14</v>
       </c>
       <c r="I33" s="17"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="53"/>
-      <c r="N33" s="53"/>
-      <c r="O33" s="53"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="52"/>
+      <c r="O33" s="52"/>
     </row>
     <row r="34" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" s="46" t="s">
@@ -2111,18 +2115,18 @@
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="23"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="56"/>
+      <c r="O34" s="56"/>
     </row>
     <row r="35" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="56">
+      <c r="B35" s="59">
         <v>13.54</v>
       </c>
       <c r="C35" s="12">
@@ -2145,16 +2149,16 @@
       <c r="I35" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="53"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="52"/>
     </row>
     <row r="36" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="38"/>
-      <c r="B36" s="56"/>
+      <c r="B36" s="59"/>
       <c r="C36" s="12"/>
       <c r="D36" s="13">
         <f>B36*C36</f>
@@ -2167,16 +2171,16 @@
         <v>14</v>
       </c>
       <c r="I36" s="17"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="53"/>
-      <c r="N36" s="53"/>
-      <c r="O36" s="53"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
+      <c r="O36" s="52"/>
     </row>
     <row r="37" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="38"/>
-      <c r="B37" s="56"/>
+      <c r="B37" s="59"/>
       <c r="C37" s="12"/>
       <c r="D37" s="13">
         <f>B37*C37</f>
@@ -2206,18 +2210,18 @@
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="I38" s="23"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="52"/>
-      <c r="L38" s="52"/>
-      <c r="M38" s="52"/>
-      <c r="N38" s="52"/>
-      <c r="O38" s="52"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="56"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="56"/>
+      <c r="O38" s="56"/>
     </row>
     <row r="39" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="56">
+      <c r="B39" s="59">
         <v>7.8</v>
       </c>
       <c r="C39" s="12">
@@ -2240,18 +2244,18 @@
       <c r="I39" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="53"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="52"/>
+      <c r="N39" s="52"/>
+      <c r="O39" s="52"/>
     </row>
     <row r="40" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B40" s="56">
+      <c r="B40" s="59">
         <v>6</v>
       </c>
       <c r="C40" s="12">
@@ -2274,18 +2278,18 @@
       <c r="I40" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
-      <c r="N40" s="53"/>
-      <c r="O40" s="53"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="52"/>
+      <c r="M40" s="52"/>
+      <c r="N40" s="52"/>
+      <c r="O40" s="52"/>
     </row>
     <row r="41" spans="1:15" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="56">
+      <c r="B41" s="59">
         <v>4.83</v>
       </c>
       <c r="C41" s="12">
@@ -2308,12 +2312,12 @@
       <c r="I41" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="53"/>
-      <c r="M41" s="53"/>
-      <c r="N41" s="53"/>
-      <c r="O41" s="53"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="52"/>
+      <c r="O41" s="52"/>
     </row>
     <row r="42" spans="1:15" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="47" t="s">
@@ -2327,31 +2331,31 @@
       <c r="G42" s="40"/>
       <c r="H42" s="40"/>
       <c r="I42" s="41"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="54"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54"/>
-      <c r="O42" s="54"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
     </row>
     <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="57">
-        <v>37.200000000000003</v>
+      <c r="B43" s="58">
+        <v>28.8</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" s="13">
         <f>B43*C43</f>
-        <v>37.200000000000003</v>
-      </c>
-      <c r="E43" s="59" t="s">
+        <v>28.8</v>
+      </c>
+      <c r="E43" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="F43" s="58" t="s">
+      <c r="F43" s="50" t="s">
         <v>108</v>
       </c>
       <c r="G43" s="37"/>
@@ -2364,6 +2368,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="J11:O11"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="J15:O15"/>
+    <mergeCell ref="J16:O16"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="J24:O24"/>
     <mergeCell ref="J40:O40"/>
     <mergeCell ref="J41:O41"/>
     <mergeCell ref="J42:O42"/>
@@ -2380,29 +2407,6 @@
     <mergeCell ref="J34:O34"/>
     <mergeCell ref="J25:O25"/>
     <mergeCell ref="J26:O26"/>
-    <mergeCell ref="J27:O27"/>
-    <mergeCell ref="J28:O28"/>
-    <mergeCell ref="J29:O29"/>
-    <mergeCell ref="J18:O18"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="J22:O22"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="J15:O15"/>
-    <mergeCell ref="J16:O16"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J7:O7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I7" r:id="rId1" location="90967A160"/>

</xml_diff>